<commit_message>
remove buggy code and make xlsx more complex with a group containing a select_multiple
</commit_message>
<xml_diff>
--- a/iaso/tests/fixtures/odk_valid_multi_select.xlsx
+++ b/iaso/tests/fixtures/odk_valid_multi_select.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -161,6 +161,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">demo_integer</t>
     </r>
@@ -173,6 +174,15 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">propriete_fonciere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">II. PROPRIERE FONCIERE ET INFRASTRUCTURE DE BASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_source_elec</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -298,8 +308,10 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -309,12 +321,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7E4BD"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -347,7 +365,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,8 +389,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,30 +410,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in 40% - Accent3" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -450,7 +476,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFD7E4BD"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -482,16 +508,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.03"/>
   </cols>
   <sheetData>
@@ -641,6 +668,39 @@
       </c>
       <c r="J9" s="0" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +725,7 @@
       <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.59"/>
@@ -674,9 +734,9 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -690,98 +750,98 @@
       <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>46</v>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>49</v>
+      <c r="B4" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>52</v>
+      <c r="B5" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
+      <c r="B6" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -806,27 +866,27 @@
       <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="18.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>65</v>
+      <c r="A1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="A2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>2020022401</v>
       </c>
     </row>

</xml_diff>